<commit_message>
disturb excel translation file cells.
</commit_message>
<xml_diff>
--- a/TestFiles/ContentTest.xlsx
+++ b/TestFiles/ContentTest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79">
   <si>
     <t>ENU</t>
   </si>
@@ -40,18 +40,6 @@
     <t>un</t>
   </si>
   <si>
-    <t>two</t>
-  </si>
-  <si>
-    <t>二</t>
-  </si>
-  <si>
-    <t>zwei</t>
-  </si>
-  <si>
-    <t>deux</t>
-  </si>
-  <si>
     <t>three</t>
   </si>
   <si>
@@ -64,28 +52,16 @@
     <t>trois</t>
   </si>
   <si>
-    <t>four</t>
-  </si>
-  <si>
-    <t>四</t>
-  </si>
-  <si>
-    <t>vier</t>
-  </si>
-  <si>
-    <t>quatre</t>
-  </si>
-  <si>
-    <t>five</t>
-  </si>
-  <si>
-    <t>五</t>
-  </si>
-  <si>
-    <t>fünf</t>
-  </si>
-  <si>
-    <t>cinq</t>
+    <t>thirteen</t>
+  </si>
+  <si>
+    <t>十三</t>
+  </si>
+  <si>
+    <t>dreizehn</t>
+  </si>
+  <si>
+    <t>treize</t>
   </si>
   <si>
     <t>six</t>
@@ -110,6 +86,78 @@
 </t>
   </si>
   <si>
+    <t>sixteen</t>
+  </si>
+  <si>
+    <t>十六.</t>
+  </si>
+  <si>
+    <t>sechszehn</t>
+  </si>
+  <si>
+    <t>seize</t>
+  </si>
+  <si>
+    <t>fifteen</t>
+  </si>
+  <si>
+    <t>十五</t>
+  </si>
+  <si>
+    <t>fünfzehn</t>
+  </si>
+  <si>
+    <t>quinze</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>四</t>
+  </si>
+  <si>
+    <t>vier</t>
+  </si>
+  <si>
+    <t>quatre</t>
+  </si>
+  <si>
+    <t>fourteen</t>
+  </si>
+  <si>
+    <t>十四。</t>
+  </si>
+  <si>
+    <t>vierzehn</t>
+  </si>
+  <si>
+    <t>quatorze</t>
+  </si>
+  <si>
+    <t>eleven</t>
+  </si>
+  <si>
+    <t>十一</t>
+  </si>
+  <si>
+    <t>elf</t>
+  </si>
+  <si>
+    <t>onze</t>
+  </si>
+  <si>
+    <t>nine</t>
+  </si>
+  <si>
+    <t>九</t>
+  </si>
+  <si>
+    <t>neun</t>
+  </si>
+  <si>
+    <t>neuf</t>
+  </si>
+  <si>
     <t>eight</t>
   </si>
   <si>
@@ -122,16 +170,52 @@
     <t>huit</t>
   </si>
   <si>
-    <t>nine</t>
-  </si>
-  <si>
-    <t>九</t>
-  </si>
-  <si>
-    <t>neun</t>
-  </si>
-  <si>
-    <t>neuf</t>
+    <t>twelve a</t>
+  </si>
+  <si>
+    <t>十 二 、\n</t>
+  </si>
+  <si>
+    <t>zwölf</t>
+  </si>
+  <si>
+    <t>douze</t>
+  </si>
+  <si>
+    <t>sev enteen.</t>
+  </si>
+  <si>
+    <t>十七 s</t>
+  </si>
+  <si>
+    <t>siebzehn</t>
+  </si>
+  <si>
+    <t>dix-sept</t>
+  </si>
+  <si>
+    <t>nin ete en.</t>
+  </si>
+  <si>
+    <t>十 九</t>
+  </si>
+  <si>
+    <t>neunzehn</t>
+  </si>
+  <si>
+    <t>dix-neuf</t>
+  </si>
+  <si>
+    <t>eighteen\n</t>
+  </si>
+  <si>
+    <t>十八</t>
+  </si>
+  <si>
+    <t>achtzehn</t>
+  </si>
+  <si>
+    <t>dix-huit</t>
   </si>
   <si>
     <t>ten</t>
@@ -146,124 +230,28 @@
     <t>dix</t>
   </si>
   <si>
-    <t>eleven</t>
-  </si>
-  <si>
-    <t>十一</t>
-  </si>
-  <si>
-    <t>elf</t>
-  </si>
-  <si>
-    <t>onze</t>
-  </si>
-  <si>
-    <t>twelve a</t>
-  </si>
-  <si>
-    <t>十 二 、\n</t>
-  </si>
-  <si>
-    <t>zwölf</t>
-  </si>
-  <si>
-    <t>douze</t>
-  </si>
-  <si>
-    <t>thirteen</t>
-  </si>
-  <si>
-    <t>十三</t>
-  </si>
-  <si>
-    <t>dreizehn</t>
-  </si>
-  <si>
-    <t>treize</t>
-  </si>
-  <si>
-    <t>fourteen</t>
-  </si>
-  <si>
-    <t>十四。</t>
-  </si>
-  <si>
-    <t>vierzehn</t>
-  </si>
-  <si>
-    <t>quatorze</t>
-  </si>
-  <si>
-    <t>fifteen</t>
-  </si>
-  <si>
-    <t>十五</t>
-  </si>
-  <si>
-    <t>fünfzehn</t>
-  </si>
-  <si>
-    <t>quinze</t>
-  </si>
-  <si>
-    <t>sixteen</t>
-  </si>
-  <si>
-    <t>十六.</t>
-  </si>
-  <si>
-    <t>sechszehn</t>
-  </si>
-  <si>
-    <t>seize</t>
-  </si>
-  <si>
-    <t>sev enteen.</t>
-  </si>
-  <si>
-    <t>十七 s</t>
-  </si>
-  <si>
-    <t>siebzehn</t>
-  </si>
-  <si>
-    <t>dix-sept</t>
-  </si>
-  <si>
-    <t>eighteen\n</t>
-  </si>
-  <si>
-    <t>十八</t>
-  </si>
-  <si>
-    <t>achtzehn</t>
-  </si>
-  <si>
-    <t>dix-huit</t>
-  </si>
-  <si>
-    <t>nin ete en.</t>
-  </si>
-  <si>
-    <t>十 九</t>
-  </si>
-  <si>
-    <t>neunzehn</t>
-  </si>
-  <si>
-    <t>dix-neuf</t>
-  </si>
-  <si>
-    <t>twe nty</t>
-  </si>
-  <si>
-    <t>二 十</t>
-  </si>
-  <si>
-    <t>zwanzig</t>
-  </si>
-  <si>
-    <t>vingt</t>
+    <t>two</t>
+  </si>
+  <si>
+    <t>二</t>
+  </si>
+  <si>
+    <t>zwei</t>
+  </si>
+  <si>
+    <t>deux</t>
+  </si>
+  <si>
+    <t>five</t>
+  </si>
+  <si>
+    <t>五</t>
+  </si>
+  <si>
+    <t>fünf</t>
+  </si>
+  <si>
+    <t>cinq</t>
   </si>
 </sst>
 </file>
@@ -271,10 +259,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -286,6 +274,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -294,22 +289,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,6 +302,90 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -333,97 +396,22 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -444,97 +432,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,79 +588,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -632,17 +620,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -664,35 +670,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -712,11 +694,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -734,148 +722,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1208,10 +1196,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33333333333333" defaultRowHeight="19" outlineLevelCol="3"/>
@@ -1286,35 +1274,35 @@
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1" spans="1:4">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" ht="22" customHeight="1" spans="1:4">
@@ -1327,7 +1315,7 @@
       <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1499,21 +1487,10 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A1:D21">
+    <sortCondition ref="D21" descending="1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>